<commit_message>
Adjusted excel + jupyter for start-up/shut-down limits
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/ammonia/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\01_input_data\01_input_raw\ammonia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4572EB0-D0E6-404F-8F12-72EDCB9F9D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D19251-0FF9-40A7-B87F-3ACD7DB13BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3930" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>Unit</t>
   </si>
@@ -161,6 +161,18 @@
   </si>
   <si>
     <t>ramp_down_Output1</t>
+  </si>
+  <si>
+    <t>start_up_Output1</t>
+  </si>
+  <si>
+    <t>start_up_Output2</t>
+  </si>
+  <si>
+    <t>shut_down_Output1</t>
+  </si>
+  <si>
+    <t>shut_down_Output2</t>
   </si>
 </sst>
 </file>
@@ -234,9 +246,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AC6" totalsRowShown="0">
-  <autoFilter ref="A1:AC6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AG6" totalsRowShown="0">
+  <autoFilter ref="A1:AG6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="33">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
@@ -255,6 +267,10 @@
     <tableColumn id="28" xr3:uid="{EBC4610B-47F0-44E3-8543-664851FC473C}" name="ramp_up_Output2"/>
     <tableColumn id="27" xr3:uid="{DC89C4F2-3857-45F2-B4A0-642F9C1613A6}" name="ramp_down_Output1"/>
     <tableColumn id="29" xr3:uid="{5A66563E-85FF-4FFA-9DB7-EAC64F37E721}" name="ramp_down_Output2"/>
+    <tableColumn id="30" xr3:uid="{98C94D50-387A-4596-96E7-17395B3AF62E}" name="start_up_Output1"/>
+    <tableColumn id="31" xr3:uid="{FF26E17F-A633-477F-A8B8-3FD0C0B88F7D}" name="start_up_Output2"/>
+    <tableColumn id="32" xr3:uid="{D45EEC70-4FBC-44FF-9E9A-E2D38C52BF94}" name="shut_down_Output1"/>
+    <tableColumn id="33" xr3:uid="{D8C88D78-E68F-45EF-8A97-7C1F84821946}" name="shut_down_Output2"/>
     <tableColumn id="9" xr3:uid="{50F936EF-D32C-4938-8FCA-291A6A3E82E6}" name="Relation_In_In"/>
     <tableColumn id="20" xr3:uid="{84C680FD-12EA-4AE2-A238-57453A3D8C12}" name="Relation_In_Out"/>
     <tableColumn id="10" xr3:uid="{ACDE4024-BCA2-4145-B3BC-1A5A08F3EA7D}" name="Relation_Out_Out"/>
@@ -621,7 +637,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AG1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -637,17 +653,17 @@
     <col min="11" max="11" width="20.08984375" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21.90625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" hidden="1" customWidth="1"/>
-    <col min="14" max="18" width="10.54296875" customWidth="1"/>
-    <col min="19" max="19" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.7265625" customWidth="1"/>
-    <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11" customWidth="1"/>
-    <col min="26" max="26" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="22" width="10.54296875" customWidth="1"/>
+    <col min="23" max="23" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="12.7265625" customWidth="1"/>
+    <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11" customWidth="1"/>
+    <col min="30" max="30" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -703,36 +719,48 @@
         <v>39</v>
       </c>
       <c r="S1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>6</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AA1" t="s">
         <v>36</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AE1" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AF1" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AG1" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>